<commit_message>
Fix(excel) read with cols error
Add example to README.md
</commit_message>
<xml_diff>
--- a/easyio/excel/tests/test.xlsx
+++ b/easyio/excel/tests/test.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11800" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="11800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -36,33 +38,47 @@
     <t>Price</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Date</t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>To kill a mocking bird</t>
+  </si>
+  <si>
+    <t>$9.9</t>
+  </si>
+  <si>
+    <t>Level-2-rack-1</t>
+  </si>
+  <si>
+    <t>Python cookbook</t>
+  </si>
+  <si>
+    <t>$12.9</t>
+  </si>
+  <si>
+    <t>Level-1-rack-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -517,148 +533,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -666,10 +682,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="24" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -991,35 +1007,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>22</v>
       </c>
     </row>
@@ -1032,80 +1057,50 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>777</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="9.84615384615385"/>
+    <col min="1" max="1" width="20.7692307692308" customWidth="1"/>
+    <col min="2" max="2" width="9.23076923076923" style="1"/>
+    <col min="3" max="3" width="16.6634615384615" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43831</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44594</v>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(excel): Close workbook if it is opened in read-only mode. docs(readme): Add excel-read-as-dict example
</commit_message>
<xml_diff>
--- a/easyio/excel/tests/test.xlsx
+++ b/easyio/excel/tests/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11800" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="11800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -26,10 +26,19 @@
     <t>Age</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Peter</t>
   </si>
   <si>
+    <t>A man</t>
+  </si>
+  <si>
     <t>Brain</t>
+  </si>
+  <si>
+    <t>A fool</t>
   </si>
   <si>
     <t>Book</t>
@@ -85,6 +94,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -92,7 +108,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -114,38 +130,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,9 +169,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,55 +215,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,181 +252,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,6 +437,69 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -457,54 +529,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -513,168 +537,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1007,15 +1016,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1025,27 +1034,36 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>45</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1059,7 +1077,7 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1072,35 +1090,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>